<commit_message>
Diary Guowei Li 01162020
</commit_message>
<xml_diff>
--- a/diaries/diary-guowei-li.xlsx
+++ b/diaries/diary-guowei-li.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="8060" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1420" yWindow="6180" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -122,6 +122,34 @@
   </si>
   <si>
     <t>&lt;how did you feel during the activity?&gt;</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jan 16th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 - 8 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revise last week's material, learn the basic strategies for code comprehension,  do an in-class practice and listen to a speech by Ping.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Understood different kinds of strategies for reading code, gained hands-on experience by doing practice, and also knew how professional programmers read code. </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>First of all, different kinds of stategies can all be used. We don't need to insist on one specific strategy when reading code. Second, it's really necessary to assign meaningful names to variables, functions and classes. It helps a lot when people try to understand your code. Last but not least,  documenting is good for everybody in your group at work.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Great. I need time to get truly familiar with what I learned this time.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -129,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +255,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -260,12 +296,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -274,9 +314,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -308,10 +345,17 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="超链接" xfId="4" builtinId="8"/>
+    <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="无色" xfId="3" builtinId="28"/>
@@ -618,7 +662,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -637,412 +681,426 @@
     <col min="1" max="7" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="21" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A4" s="5" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="21" customHeight="1">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A6" s="5" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A9" s="11" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="52">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="52">
+      <c r="A10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="117">
+      <c r="A11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13"/>
-    </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="13"/>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="13"/>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="13"/>
-    </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="13"/>
-    </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="13"/>
-    </row>
-    <row r="37" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="13"/>
-    </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="13"/>
-    </row>
-    <row r="39" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="13"/>
+    <row r="13" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" spans="1:7" ht="13">
       <c r="A40" s="1"/>

</xml_diff>

<commit_message>
diary guowei li 01232020
</commit_message>
<xml_diff>
--- a/diaries/diary-guowei-li.xlsx
+++ b/diaries/diary-guowei-li.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="6180" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="7600" yWindow="4500" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -150,6 +150,34 @@
   </si>
   <si>
     <t>Great. I need time to get truly familiar with what I learned this time.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jan 23rd, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 - 8 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revise last week's material, learn mental models and externalizing them, get familiar with UML class diagrams, do an in-class practice and have a face-to-face communication with Alegria.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Knew what mental models and UML class diagrams are and gave a try to make UML diagrams with the simpleUML plugin. What's more, learned about what a programmer's life (basically her way to read code) is like from Alegria's narrate.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">UML class diagrams help a lot when programmers try to figure out logical relationships among many java components by visualize them clearly. </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>It's about the time to devote more time to our group project and really dive into it.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -296,12 +324,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -349,13 +378,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="超链接" xfId="4" builtinId="8"/>
     <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="无色" xfId="3" builtinId="28"/>
@@ -662,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -672,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -836,27 +866,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="13">
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="78">
       <c r="A12" s="11" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="3" customFormat="1" ht="13">
@@ -869,13 +899,27 @@
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
+      <c r="A14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" ht="13">
       <c r="A15" s="11"/>

</xml_diff>

<commit_message>
Diary guowei li 01302020 (#254)
* delete the annoying .DS_Store file

* diary guowei li 01302020

* Delete ~$diary-guowei-li.xlsx

Co-authored-by: oscarli97 <34699090+oscarli97@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/diaries/diary-guowei-li.xlsx
+++ b/diaries/diary-guowei-li.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="4500" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1620" yWindow="3480" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -178,6 +178,34 @@
   </si>
   <si>
     <t>It's about the time to devote more time to our group project and really dive into it.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jan 30th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 - 8 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revise last week's material, learn 3 key expert practices, get to know differences between structural and behavioral models, dive deeper into UML diagrams and  do an in-class practice.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Formed the idea of what practices I should apply when work as a professional programmer. Understood main differences between structural and behavioral models,</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Working as a programmer isn't just about mastering coding techniques. It's also about team spirit, being clear about your goals and  many other things.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Now I have already understood the importance of teamwork. It's time-efficient when group members worked together.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -324,12 +352,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -378,7 +407,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="超链接" xfId="4" builtinId="8"/>
     <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
@@ -386,6 +415,7 @@
     <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="无色" xfId="3" builtinId="28"/>
@@ -692,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -889,61 +919,75 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
+    <row r="13" spans="1:7" s="3" customFormat="1" ht="78">
+      <c r="A13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G15" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-    </row>
     <row r="16" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="12"/>
@@ -952,7 +996,7 @@
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="10"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="12"/>
@@ -979,7 +1023,7 @@
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="12"/>
@@ -1137,14 +1181,14 @@
       <c r="F38" s="11"/>
       <c r="G38" s="12"/>
     </row>
-    <row r="39" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="12"/>
+    <row r="39" spans="1:7" ht="13">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" ht="13">
       <c r="A40" s="1"/>
@@ -1910,15 +1954,6 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="2"/>
-    </row>
-    <row r="125" spans="1:7" ht="13">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
-      <c r="G125" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update diary entries from Feb 14th to Feb 20th
</commit_message>
<xml_diff>
--- a/diaries/diary-guowei-li.xlsx
+++ b/diaries/diary-guowei-li.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="3480" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="2700" yWindow="2720" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -185,6 +185,26 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
+    <t>Revise last week's material, learn 3 key expert practices, get to know differences between structural and behavioral models, dive deeper into UML diagrams and  do an in-class practice.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Formed the idea of what practices I should apply when work as a professional programmer. Understood main differences between structural and behavioral models,</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Working as a programmer isn't just about mastering coding techniques. It's also about team spirit, being clear about your goals and  many other things.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Now I have already understood the importance of teamwork. It's time-efficient when group members worked together.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feb 6th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
     <t>5 - 8 pm</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -193,19 +213,63 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Revise last week's material, learn 3 key expert practices, get to know differences between structural and behavioral models, dive deeper into UML diagrams and  do an in-class practice.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Formed the idea of what practices I should apply when work as a professional programmer. Understood main differences between structural and behavioral models,</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Working as a programmer isn't just about mastering coding techniques. It's also about team spirit, being clear about your goals and  many other things.</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Now I have already understood the importance of teamwork. It's time-efficient when group members worked together.</t>
+    <t>Feb 13th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feb 20th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 - 8 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revise last week's material, master 3 more key expert practices, learn what mental simulation is and do in-class practice.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Did several mental simulation practices using various examples. Explored by what rules Blinky moves.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I made a mistake when I was doing mental simulation on one of those examples. In this example, the comment line is not consistent with the real code below it. I judged too quickly about what the code does. That was when I really realized that we should go slow, be skeptical and only rely on our observations and analysis.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>All things about coding is like art. You need to not only master techniques but also have a keen heart that can be dedicated to what you do and quickly uncover the secret for how to do a good job from observation.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reveal class survey results, revise last week's material, master 3 more key expert practices and learn how to form a big picture of a software.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned how to form a big picture of a software by analyzing stakeholders, key developers and functionality of it. </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>There are many aspects worth analyzing of a software. Valuable information can be obtained from its documentation, github page, website and so on.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>The course is completely different from courses I used to have. It seems to focus mainly on the practical side of programming.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revise last week's material, master 3 more key expert practices learn about the architecture and social context of a software.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learned ways of how to group components in a software to oueline its architecture. Knew more aspects of a software like the social context, the ideal process of contributing to a github project.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We've learned 12 key expert practices. Honestly I can understand their meaning from Andre's instruction but I have no idea how those expert practices would change my mindset since I haven't really applied many of them so far. Maybe more experience would be a natural trigger for me to digest them faster.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nothing much.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -732,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -924,82 +988,124 @@
         <v>42</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="G13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="11" t="s">
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="117">
+      <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="C14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="52">
       <c r="A15" s="11" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="104">
+      <c r="A16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" ht="13">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="10"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" ht="13">
       <c r="A19" s="11"/>

</xml_diff>

<commit_message>
Add diary entries from Feb 23rd to Mar 1st
</commit_message>
<xml_diff>
--- a/diaries/diary-guowei-li.xlsx
+++ b/diaries/diary-guowei-li.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2720" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="4840" yWindow="2040" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -270,6 +270,109 @@
   </si>
   <si>
     <t>Nothing much.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dongxin Xiang, Jing Chen</t>
+  </si>
+  <si>
+    <t>Feb 27th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 - 8 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Revise last week's material, master 3 more key practices, learn various kinds of design patterns, </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 am - 10 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mar 1st, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 am - 6 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dongxin Xiang, Jing Chen</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feb 23rd, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feb 19th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 am - 5 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Identify five different design patterns that are used in Omni-Notes, provide an example per pattern and explain benefits. Code up first issue and submit a pull request.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found five different patterns in Omni-Notes, including adapter, async method invocation, private class data, factory kit and mvc. Fixed an open issue #663 (Change the duration of a crouton message) and submitted our first pull request..</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We learned a lot about advantages &amp; disadvantages of each pattern. On top of that, we were thinking about our secong issue to solve.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>A busy day passed so fast.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expressed my opinion about last homework. Learned some oftware design patterns and categories of software design pattern.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patterns are very practical for us to use to solve a software designing problem. They have been proved to be correct and efficient. We could save a lot of time if we use them when solving software designing problems.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I've seen many of these patterns but I didn't pay attention and dive deeper into them. I am eager to learn more of them so that they will help me with my professional work in the future.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dive into Omni-Notes by recording its state and exploring its architecture, try to  find five "interesting" pull request and five"interesting" open issues.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Looked through a huge amount of resources, getting a big collection of information about Omni-Notes. Found five  "interesting" pull request and five"interesting" open issues, clearly stating them in our homework.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We learned a lot from "intersting" open issues and pull requests. One point that I may never forget is that contributors need to obey many rules to contribute to a project. Those rules include coding style, unit tests and so on.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I'm becoming more and more professional!</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Construct a big picture of Omni-Notes by exploring its stakeholders, key developers and functionality.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Looked through a lot of resources including Omni-Notes' github website and Google Play store, finding what we though were important and formed a big picture of this software.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>A software has so many aspacts to learn about.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -416,12 +519,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -471,7 +577,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="14">
     <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="超链接" xfId="4" builtinId="8"/>
     <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
@@ -480,6 +586,9 @@
     <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="无色" xfId="3" builtinId="28"/>
@@ -786,7 +895,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -794,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1052,93 +1161,149 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="104">
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="65">
       <c r="A16" s="11" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="13">
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="104">
+      <c r="A17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="78">
       <c r="A18" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" ht="78">
+      <c r="A19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" ht="91">
+      <c r="A20" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" ht="13">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="12"/>
@@ -1147,7 +1312,7 @@
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="12"/>
@@ -1287,32 +1452,32 @@
       <c r="F38" s="11"/>
       <c r="G38" s="12"/>
     </row>
-    <row r="39" spans="1:7" ht="13">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" ht="13">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="13">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="2"/>
+    <row r="39" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:7" ht="13">
       <c r="A42" s="1"/>
@@ -2060,6 +2225,33 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="2"/>
+    </row>
+    <row r="125" spans="1:7" ht="13">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="2"/>
+    </row>
+    <row r="126" spans="1:7" ht="13">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="2"/>
+    </row>
+    <row r="127" spans="1:7" ht="13">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add diary entries from Mar 10th to 16th
</commit_message>
<xml_diff>
--- a/diaries/diary-guowei-li.xlsx
+++ b/diaries/diary-guowei-li.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="2040" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="3400" yWindow="120" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="119">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -373,6 +373,119 @@
   </si>
   <si>
     <t>A software has so many aspacts to learn about.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mar 5th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mar 12th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mar 14th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feb, 9th, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feb, 2nd, 2020</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 - 8 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 am - 3 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 am - 5 pm</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prepare and print a UML class diagram for Omni-Notes, decide upon two different features and highlight in the UML class diagram where those two features are implemented and record on paper how we find where those features are implemented</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chose search and reminder to explore, found where they are implemented and wrote our first report.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We applied systematic comprehension strategy to read code which was really efficient. We realized it is important to master such techiniques on top of  learning how to code.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>It's been great diving into an open source program, which I never did before.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decide upon two features that are essential in Omni-Notes and imagine that each of the two features will need to undergo some kind of change to be implemented by someone else.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chose search and note creation as essential features and prepared a packet, per feature, that would assist that other person in understanding where the feature is located, what other parts of the system may be relevant, and how those parts are relevant.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">For Omni-Notes, essential features should be features which ensure Omni-Notes is a note taking app in nature. </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I feel a sense of accomplishment since we prepared a big packet for people to understand the system.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revise last week's material, master 3 more key practices, learn about concepts of testing.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solidate what I learned from 261P in the context of 265P by doing the in-class practice.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andre showed us several reflective questions on the slides. I thought we should really ask ourselves these questions before writing test cases.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excited coz it's nearly the end of the quarter.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code up our second issue, find three interesting test cases and write three new test cases for Omni-Notes.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed the second issue - implementing seraching in a note feature. Dived into existing test cases and added some new test cases. From our experience of coding up the second open issue, we gained deeper understandings of Omni-Notes.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We met techniques that we never met before. Omni-Notes uses the BindView annotations to bind layout components to corresponding variables in DetailFragment upon their declarations. Later we learned that the BindView annotations are from Butterknife - an Android library for view injections. The system also applies the SuppressLint annotations, which are used by the Android Lint tool, to suppress all warnings that would tell you if you are using any API introduced after your minSdkVersion.
+In addition, it is really important to follow all the rules such as the coding style to make acceptable modifications to the system. Some contributors actually made valuable contributions to the system but their pull requests could not easily get merged because they somehow violated rules, which we explored in detail in homework 4. Code is maintainable and readable only when all of it follows a standard.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revise last week's material, master 3 more key practices, learned miscellaneous topics.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self-learned the content of lectur 10, got to know some advanced techniques used in software engineering.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>There's a lot to learn in software engineering. There are many existing techniques and new techniques keep emerging.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>During the last lecture time, what I was thinking was I appreciated Andre's lectures and Kaj's instructions.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>The journey of exploring Omni-Notes comes to an end. We are happy that we actually did some contributions to the project.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -519,12 +632,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -577,9 +693,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="17">
+    <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="差" xfId="2" builtinId="27"/>
-    <cellStyle name="超链接" xfId="4" builtinId="8"/>
+    <cellStyle name="无色" xfId="3" builtinId="28"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
@@ -589,9 +707,10 @@
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
-    <cellStyle name="无色" xfId="3" builtinId="28"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="4" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -895,7 +1014,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -903,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1115,32 +1234,32 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="117">
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="91">
       <c r="A14" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="117">
+      <c r="A15" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="52">
-      <c r="A15" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>48</v>
@@ -1149,206 +1268,276 @@
         <v>49</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="65">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="91">
       <c r="A16" s="11" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" ht="104">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="52">
       <c r="A17" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="78">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="65">
       <c r="A18" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" ht="104">
+      <c r="A19" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" ht="78">
+      <c r="A20" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" ht="78">
-      <c r="A19" s="11" t="s">
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="78">
+      <c r="A21" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" ht="91">
-      <c r="A20" s="11" t="s">
+    <row r="22" spans="1:7" s="3" customFormat="1" ht="91">
+      <c r="A22" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G22" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A21" s="11" t="s">
+    <row r="23" spans="1:7" s="3" customFormat="1" ht="52">
+      <c r="A23" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="52">
+      <c r="A24" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1" ht="312">
+      <c r="A25" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A26" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G26" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" ht="13">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" s="3" customFormat="1" ht="13">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="12"/>
@@ -1357,7 +1546,7 @@
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="12"/>
@@ -1479,50 +1668,50 @@
       <c r="F41" s="11"/>
       <c r="G41" s="12"/>
     </row>
-    <row r="42" spans="1:7" ht="13">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" ht="13">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="13">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" ht="13">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" ht="13">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="2"/>
+    <row r="42" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" spans="1:7" s="3" customFormat="1" ht="13">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="12"/>
     </row>
     <row r="47" spans="1:7" ht="13">
       <c r="A47" s="1"/>
@@ -2252,6 +2441,51 @@
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="2"/>
+    </row>
+    <row r="128" spans="1:7" ht="13">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="2"/>
+    </row>
+    <row r="129" spans="1:7" ht="13">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="1:7" ht="13">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="2"/>
+    </row>
+    <row r="131" spans="1:7" ht="13">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="2"/>
+    </row>
+    <row r="132" spans="1:7" ht="13">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>